<commit_message>
SPI & I2C added
</commit_message>
<xml_diff>
--- a/slides/Interfacing.xlsx
+++ b/slides/Interfacing.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t xml:space="preserve">Topic </t>
   </si>
@@ -85,9 +85,6 @@
     <t>Interrupt</t>
   </si>
   <si>
-    <t>relay,buzzer,Alarm app, DIO Driver with layered architecture</t>
-  </si>
-  <si>
     <t>External Interrupt</t>
   </si>
   <si>
@@ -98,16 +95,69 @@
   </si>
   <si>
     <t>Write GPIO Driver for Tiva C</t>
+  </si>
+  <si>
+    <t>https://github.com/Mohamedsaied8/AMIT_labs/blob/master/slides/computer%20architecture%20ver%201.3.pdf</t>
+  </si>
+  <si>
+    <t>https://github.com/Mohamedsaied8/AMIT_labs/blob/master/slides/embedded%20C.pptx</t>
+  </si>
+  <si>
+    <t>https://github.com/Mohamedsaied8/AMIT_labs/blob/master/slides/DIO_Interfacing.pptx</t>
+  </si>
+  <si>
+    <t>DIO_Layered Arch.</t>
+  </si>
+  <si>
+    <t>DIO Driver with Layered Architecture</t>
+  </si>
+  <si>
+    <t>https://github.com/Mohamedsaied8/AMIT_labs/blob/master/slides/GPIO.pptx</t>
+  </si>
+  <si>
+    <t>relay,buzzer,Alarm app</t>
+  </si>
+  <si>
+    <t>https://github.com/Mohamedsaied8/AMIT_labs/blob/master/slides/LCD.pptx</t>
+  </si>
+  <si>
+    <t>https://github.com/Mohamedsaied8/AMIT_labs/blob/master/slides/Interrupt.pptx</t>
+  </si>
+  <si>
+    <t>https://github.com/Mohamedsaied8/AMIT_labs/blob/master/slides/ADC.pptx</t>
+  </si>
+  <si>
+    <t>https://github.com/Mohamedsaied8/AMIT_labs/blob/master/slides/UART.pptx</t>
+  </si>
+  <si>
+    <t>keypad</t>
+  </si>
+  <si>
+    <t>KP layered Arch, kP with LCD app</t>
+  </si>
+  <si>
+    <t>https://github.com/Mohamedsaied8/AMIT_labs/blob/master/slides/Keypad.pptx</t>
+  </si>
+  <si>
+    <t>https://github.com/Mohamedsaied8/AMIT_labs/blob/master/slides/Timer.pptx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -130,13 +180,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -439,17 +492,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.85546875" customWidth="1"/>
     <col min="2" max="2" width="54.42578125" customWidth="1"/>
-    <col min="3" max="3" width="57.42578125" customWidth="1"/>
+    <col min="3" max="3" width="104" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -470,6 +523,9 @@
       <c r="B2" t="s">
         <v>3</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -478,97 +534,151 @@
       <c r="B3" t="s">
         <v>7</v>
       </c>
+      <c r="C3" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>33</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>31</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>9</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>23</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>24</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>15</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>21</v>
       </c>
-      <c r="B14" t="s">
-        <v>27</v>
+      <c r="B16" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="https://github.com/Mohamedsaied8/AMIT_labs/blob/master/slides/computer architecture ver 1.3.pdf"/>
+    <hyperlink ref="C3" r:id="rId2" display="https://github.com/Mohamedsaied8/AMIT_labs/blob/master/slides/embedded C.pptx"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C6" r:id="rId5"/>
+    <hyperlink ref="C8" r:id="rId6"/>
+    <hyperlink ref="C7" r:id="rId7"/>
+    <hyperlink ref="C9" r:id="rId8"/>
+    <hyperlink ref="C12" r:id="rId9"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>